<commit_message>
eliminación de fase en el informe y esquema.
Signed-off-by: icarvajal.cuartas <icarvajal.cuartas@udea.edu.co>
</commit_message>
<xml_diff>
--- a/Esquema.xlsx
+++ b/Esquema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabella\OneDrive\Documentos\ud\InformaticaII\Rep.local\desafio1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7448B15-BA4E-48CB-80CA-0A43A51D4C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF82B8E-746A-4DA6-9A8D-189C754A9144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="297" xr2:uid="{92D86959-2661-48BC-8F7D-A5C19EDBEBA6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>Resp.</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>float frecuencia = 0;</t>
-  </si>
-  <si>
-    <t>float fase = 0;</t>
   </si>
   <si>
     <t>Inv</t>
@@ -195,28 +192,28 @@
     <t>Análisis de datos</t>
   </si>
   <si>
-    <t xml:space="preserve">void analisis_senal(int tipoSenal, float &amp;amplitud, float &amp;frecuencia, float &amp;fase) </t>
-  </si>
-  <si>
     <t>int valorMax;int valorMin;unsigned long tiempoMax;unsigned long tiempoAnteriorPico;bool primerPico = true;</t>
   </si>
   <si>
-    <t>int tipoSenal1 =0; float fase = 0;float amplitud = 0;float frecuencia = 0;</t>
-  </si>
-  <si>
     <t>3.5</t>
   </si>
   <si>
     <t>Liberación</t>
   </si>
   <si>
-    <t xml:space="preserve">tiposenal(tipoSenal1); analisis_senal(tipoSenal1, amplitud, frecuencia, fase);void liberacion() </t>
-  </si>
-  <si>
     <t xml:space="preserve">void liberacion() </t>
   </si>
   <si>
     <t>Const int filas=220;int** matriz;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiposenal(tipoSenal1); analisis_senal(tipoSenal1, amplitud, frecuencia);void liberacion() </t>
+  </si>
+  <si>
+    <t xml:space="preserve">void analisis_senal(int tipoSenal, float &amp;amplitud, float &amp;frecuencia) </t>
+  </si>
+  <si>
+    <t>int tipoSenal1 =0;float amplitud = 0;float frecuencia = 0;</t>
   </si>
 </sst>
 </file>
@@ -328,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -369,9 +366,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -379,9 +373,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -411,49 +402,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -568,16 +516,59 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -594,7 +585,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44874B67-ABEF-4782-999E-4A9D00927B86}" name="Tabla2" displayName="Tabla2" ref="A1:H23" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44874B67-ABEF-4782-999E-4A9D00927B86}" name="Tabla2" displayName="Tabla2" ref="A1:H23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
   <autoFilter ref="A1:H23" xr:uid="{44874B67-ABEF-4782-999E-4A9D00927B86}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -606,14 +597,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8F6D8C33-19DD-4C4D-A1E0-A50B7A290AC8}" name="Resp." dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{F992B20F-4810-484E-A8A5-95576B214CD4}" name="No. " dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{7603B813-4868-4B83-92EC-14A84ED32E4B}" name="Momento" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{5507F2EC-0D05-4505-A677-F568AD4A050C}" name="Funciones" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{57D3616B-FD8E-4599-97F5-7C37F4A9E08B}" name="Variables " dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{A979D5BF-E3FA-44BF-8EB9-42A87DDE4BA4}" name="Variables conjunto" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{AEEE3C24-E128-44B6-9101-6ADEDB4BBFB7}" name="Entradas/salidas" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{DF0840E0-37D1-40EA-95DE-3F3A2000BB31}" name="Inv" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8F6D8C33-19DD-4C4D-A1E0-A50B7A290AC8}" name="Resp." dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F992B20F-4810-484E-A8A5-95576B214CD4}" name="No. " dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7603B813-4868-4B83-92EC-14A84ED32E4B}" name="Momento" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5507F2EC-0D05-4505-A677-F568AD4A050C}" name="Funciones" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{57D3616B-FD8E-4599-97F5-7C37F4A9E08B}" name="Variables " dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A979D5BF-E3FA-44BF-8EB9-42A87DDE4BA4}" name="Variables conjunto" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{AEEE3C24-E128-44B6-9101-6ADEDB4BBFB7}" name="Entradas/salidas" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{DF0840E0-37D1-40EA-95DE-3F3A2000BB31}" name="Inv" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -939,7 +930,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,15 +968,15 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="17"/>
+        <v>39</v>
+      </c>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -1004,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="9"/>
-      <c r="I2" s="17"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -1017,11 +1008,11 @@
         <v>11</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="17"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1030,9 +1021,9 @@
         <v>12</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1055,13 +1046,13 @@
         <v>9</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="17"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1080,11 +1071,11 @@
         <v>9</v>
       </c>
       <c r="H6" s="9"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="4" t="s">
@@ -1093,7 +1084,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="127.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1118,15 +1109,15 @@
         <v>9</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1147,7 +1138,7 @@
       <c r="H9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="17"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -1164,11 +1155,11 @@
         <v>29</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="17"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="5"/>
       <c r="D11" s="12"/>
       <c r="E11" s="4" t="s">
@@ -1177,15 +1168,15 @@
       <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1206,7 +1197,7 @@
       <c r="H12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="17"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1221,64 +1212,64 @@
         <v>34</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="17"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="20" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="17"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="16"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="5"/>
       <c r="D15" s="12"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" ht="126" x14ac:dyDescent="0.25">
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="17"/>
+        <v>55</v>
+      </c>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1291,7 +1282,7 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="17"/>
+      <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -1299,12 +1290,10 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="17"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1317,99 +1306,99 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="17"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="17"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="E21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="22" t="s">
+      <c r="F22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="C23" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="D23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="21" t="s">
+      <c r="E23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="17"/>
+      <c r="G23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>